<commit_message>
0.5 en 0.75 toegevoegd
</commit_message>
<xml_diff>
--- a/8p361-project-imaging-master/Main project/resnet dropout layers accuracy.xlsx
+++ b/8p361-project-imaging-master/Main project/resnet dropout layers accuracy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/j_f_peeters_student_tue_nl/Documents/Desktop/Year 3/Q3/8P361!/BIA-group-1/8p361-project-imaging-master/Main project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A3F1A87-AFE5-4D3B-A890-2CEE9B1AEBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{0A3F1A87-AFE5-4D3B-A890-2CEE9B1AEBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DC080A9-45F5-47BF-9314-57E68E6A5E66}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="1830" windowWidth="19440" windowHeight="14880" xr2:uid="{688B92CD-39F7-412F-9814-75A1BCFF03B5}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{688B92CD-39F7-412F-9814-75A1BCFF03B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Dropout</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Val Loss</t>
+  </si>
+  <si>
+    <t>0.4799</t>
+  </si>
+  <si>
+    <t>0.6066</t>
   </si>
 </sst>
 </file>
@@ -419,7 +425,7 @@
   <dimension ref="A2:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,10 +472,22 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>1.2110000000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>0.69430000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>